<commit_message>
Update as of March 8, 2025 at 10:00 AM
</commit_message>
<xml_diff>
--- a/res/excel/cbm_bases/cbm_data.xlsx
+++ b/res/excel/cbm_bases/cbm_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldri\OneDrive\Desktop\Nikka System\WLP_Automation-v7\res\excel\cbm_bases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldri\OneDrive\Desktop\WLP_Automation-v5\res\excel\cbm_bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4303D1AF-DCA0-409C-AAEA-327FEC28866A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C5592D-9652-49E3-B25D-908FA645E875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C49C2D19-4C10-4704-A717-9498010E271E}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>